<commit_message>
Adding December hours from Consultants
</commit_message>
<xml_diff>
--- a/Asset Registry System (ARS)/DaSSCo ARS Phase 3 work status overview_20241211.xlsx
+++ b/Asset Registry System (ARS)/DaSSCo ARS Phase 3 work status overview_20241211.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumni-my.sharepoint.com/personal/btw897_ku_dk/Documents/DaSSCo-Tranche-1-work/Asset Registry System (ARS)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{C50839E1-8DEC-4509-A440-77E90DB3D3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0F73988-4B43-496B-825E-CC5DBA90EA72}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{C50839E1-8DEC-4509-A440-77E90DB3D3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{039ACD72-F708-468E-9C51-7D6F2F36E54D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" xr2:uid="{D8303F33-A3AC-4B5D-B105-B60CD2BFE9AD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D8303F33-A3AC-4B5D-B105-B60CD2BFE9AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -913,7 +913,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1364,10 +1364,10 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1698,13 +1698,25 @@
       <c r="A14" t="s">
         <v>33</v>
       </c>
+      <c r="B14">
+        <v>35</v>
+      </c>
+      <c r="I14">
+        <v>42</v>
+      </c>
+      <c r="K14">
+        <v>8</v>
+      </c>
       <c r="M14" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="N14" s="1">
+        <v>85</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>